<commit_message>
Began adding support for margin checks
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\file_sys\work\workspace\osrs_stocks_12_30\osrs_stocks-master\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8A7A41-0885-4F51-853C-0AAF4A1D8CF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -70,7 +76,7 @@
     <t>test1</t>
   </si>
   <si>
-    <t>None</t>
+    <t>aborted</t>
   </si>
   <si>
     <t>test2</t>
@@ -110,18 +116,56 @@
 </t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
     <t xml:space="preserve">Very fast
 </t>
   </si>
   <si>
-    <t>aborted</t>
+    <t xml:space="preserve">ueoaueoa
+</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ueoa
+</t>
+  </si>
+  <si>
+    <t>Anglerfish</t>
+  </si>
+  <si>
+    <t>Yanillian hops</t>
+  </si>
+  <si>
+    <t>Toxic blowpipe (empty)</t>
+  </si>
+  <si>
+    <t>Tome of fire (empty)</t>
+  </si>
+  <si>
+    <t>Devout boots</t>
+  </si>
+  <si>
+    <t>Amulet of fury</t>
+  </si>
+  <si>
+    <t>Dharok's greataxe</t>
+  </si>
+  <si>
+    <t>Zulrah's scales</t>
+  </si>
+  <si>
+    <t>Divine super combat potion(4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +202,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -204,7 +256,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,9 +288,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,6 +340,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -445,14 +533,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -539,26 +632,26 @@
       <c r="K2">
         <v>15</v>
       </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" t="s">
-        <v>18</v>
+      <c r="L2">
+        <v>2019</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>31</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>59</v>
       </c>
       <c r="Q2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -592,26 +685,26 @@
       <c r="K3">
         <v>15</v>
       </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>18</v>
+      <c r="L3">
+        <v>2019</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>31</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>59</v>
       </c>
       <c r="Q3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -645,26 +738,26 @@
       <c r="K4">
         <v>15</v>
       </c>
-      <c r="L4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" t="s">
-        <v>18</v>
+      <c r="L4">
+        <v>2019</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
+      </c>
+      <c r="N4">
+        <v>31</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>59</v>
       </c>
       <c r="Q4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -698,26 +791,26 @@
       <c r="K5">
         <v>15</v>
       </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" t="s">
-        <v>18</v>
+      <c r="L5">
+        <v>2019</v>
+      </c>
+      <c r="M5">
+        <v>12</v>
+      </c>
+      <c r="N5">
+        <v>31</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>59</v>
       </c>
       <c r="Q5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -751,26 +844,26 @@
       <c r="K6">
         <v>15</v>
       </c>
-      <c r="L6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" t="s">
-        <v>18</v>
+      <c r="L6">
+        <v>2019</v>
+      </c>
+      <c r="M6">
+        <v>12</v>
+      </c>
+      <c r="N6">
+        <v>31</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>59</v>
       </c>
       <c r="Q6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -823,7 +916,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -876,7 +969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -929,7 +1022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -982,7 +1075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1035,7 +1128,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1070,25 +1163,25 @@
         <v>13</v>
       </c>
       <c r="L12" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="M12" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="N12" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="O12" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="P12" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="Q12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1105,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G13">
         <v>2019</v>
@@ -1138,7 +1231,693 @@
         <v>15</v>
       </c>
       <c r="Q13" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>1000</v>
+      </c>
+      <c r="D14">
+        <v>1200</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14">
+        <v>2019</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="I14">
+        <v>30</v>
+      </c>
+      <c r="J14">
+        <v>21</v>
+      </c>
+      <c r="K14">
+        <v>27</v>
+      </c>
+      <c r="L14">
+        <v>2019</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <v>30</v>
+      </c>
+      <c r="O14">
+        <v>21</v>
+      </c>
+      <c r="P14">
+        <v>28</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>1004</v>
+      </c>
+      <c r="D15">
+        <v>1008</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15">
+        <v>2019</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <v>30</v>
+      </c>
+      <c r="J15">
+        <v>21</v>
+      </c>
+      <c r="K15">
+        <v>34</v>
+      </c>
+      <c r="L15">
+        <v>2019</v>
+      </c>
+      <c r="M15">
+        <v>12</v>
+      </c>
+      <c r="N15">
+        <v>30</v>
+      </c>
+      <c r="O15">
+        <v>21</v>
+      </c>
+      <c r="P15">
+        <v>42</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>1100</v>
+      </c>
+      <c r="D16">
+        <v>1101</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16">
+        <v>2019</v>
+      </c>
+      <c r="H16">
+        <v>12</v>
+      </c>
+      <c r="I16">
+        <v>30</v>
+      </c>
+      <c r="J16">
+        <v>21</v>
+      </c>
+      <c r="K16">
+        <v>42</v>
+      </c>
+      <c r="L16">
+        <v>2019</v>
+      </c>
+      <c r="M16">
+        <v>12</v>
+      </c>
+      <c r="N16">
+        <v>30</v>
+      </c>
+      <c r="O16">
+        <v>21</v>
+      </c>
+      <c r="P16">
+        <v>44</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>1906</v>
+      </c>
+      <c r="D17">
+        <v>1917</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17">
+        <v>2019</v>
+      </c>
+      <c r="H17">
+        <v>12</v>
+      </c>
+      <c r="I17">
+        <v>31</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>49</v>
+      </c>
+      <c r="L17">
+        <v>2019</v>
+      </c>
+      <c r="M17">
+        <v>12</v>
+      </c>
+      <c r="N17">
+        <v>31</v>
+      </c>
+      <c r="O17">
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <v>51</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18">
+        <v>995</v>
+      </c>
+      <c r="D18">
+        <v>1005</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18">
+        <v>2019</v>
+      </c>
+      <c r="H18">
+        <v>12</v>
+      </c>
+      <c r="I18">
+        <v>31</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>50</v>
+      </c>
+      <c r="L18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" t="s">
+        <v>31</v>
+      </c>
+      <c r="O18" t="s">
+        <v>31</v>
+      </c>
+      <c r="P18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>4007343</v>
+      </c>
+      <c r="D19">
+        <v>4049000</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <v>2019</v>
+      </c>
+      <c r="H19">
+        <v>12</v>
+      </c>
+      <c r="I19">
+        <v>31</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>51</v>
+      </c>
+      <c r="L19">
+        <v>2019</v>
+      </c>
+      <c r="M19">
+        <v>12</v>
+      </c>
+      <c r="N19">
+        <v>31</v>
+      </c>
+      <c r="O19">
+        <v>5</v>
+      </c>
+      <c r="P19">
+        <v>31</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20">
+        <v>1052745</v>
+      </c>
+      <c r="D20">
+        <v>1098412</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20">
+        <v>2019</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+      <c r="I20">
+        <v>31</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>54</v>
+      </c>
+      <c r="L20">
+        <v>2019</v>
+      </c>
+      <c r="M20">
+        <v>12</v>
+      </c>
+      <c r="N20">
+        <v>31</v>
+      </c>
+      <c r="O20">
+        <v>6</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21">
+        <v>1039</v>
+      </c>
+      <c r="D21">
+        <v>1049</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21">
+        <v>2019</v>
+      </c>
+      <c r="H21">
+        <v>12</v>
+      </c>
+      <c r="I21">
+        <v>31</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>55</v>
+      </c>
+      <c r="L21" t="s">
+        <v>31</v>
+      </c>
+      <c r="M21" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" t="s">
+        <v>31</v>
+      </c>
+      <c r="O21" t="s">
+        <v>31</v>
+      </c>
+      <c r="P21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>985123</v>
+      </c>
+      <c r="D22">
+        <v>1030000</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22">
+        <v>2019</v>
+      </c>
+      <c r="H22">
+        <v>12</v>
+      </c>
+      <c r="I22">
+        <v>31</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>57</v>
+      </c>
+      <c r="L22" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" t="s">
+        <v>31</v>
+      </c>
+      <c r="N22" t="s">
+        <v>31</v>
+      </c>
+      <c r="O22" t="s">
+        <v>31</v>
+      </c>
+      <c r="P22" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23">
+        <v>1862000</v>
+      </c>
+      <c r="D23">
+        <v>1897000</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23">
+        <v>2019</v>
+      </c>
+      <c r="H23">
+        <v>12</v>
+      </c>
+      <c r="I23">
+        <v>31</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <v>58</v>
+      </c>
+      <c r="L23" t="s">
+        <v>31</v>
+      </c>
+      <c r="M23" t="s">
+        <v>31</v>
+      </c>
+      <c r="N23" t="s">
+        <v>31</v>
+      </c>
+      <c r="O23" t="s">
+        <v>31</v>
+      </c>
+      <c r="P23" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24">
+        <v>757103</v>
+      </c>
+      <c r="D24">
+        <v>764000</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24">
+        <v>2019</v>
+      </c>
+      <c r="H24">
+        <v>12</v>
+      </c>
+      <c r="I24">
+        <v>31</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <v>36</v>
+      </c>
+      <c r="L24" t="s">
+        <v>31</v>
+      </c>
+      <c r="M24" t="s">
+        <v>31</v>
+      </c>
+      <c r="N24" t="s">
+        <v>31</v>
+      </c>
+      <c r="O24" t="s">
+        <v>31</v>
+      </c>
+      <c r="P24" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25">
+        <v>200</v>
+      </c>
+      <c r="D25">
+        <v>202</v>
+      </c>
+      <c r="E25">
+        <v>30</v>
+      </c>
+      <c r="G25">
+        <v>2019</v>
+      </c>
+      <c r="H25">
+        <v>12</v>
+      </c>
+      <c r="I25">
+        <v>31</v>
+      </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>58</v>
+      </c>
+      <c r="L25">
+        <v>2019</v>
+      </c>
+      <c r="M25">
+        <v>12</v>
+      </c>
+      <c r="N25">
+        <v>31</v>
+      </c>
+      <c r="O25">
+        <v>6</v>
+      </c>
+      <c r="P25">
+        <v>20</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26">
+        <v>15624</v>
+      </c>
+      <c r="D26">
+        <v>15764</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26">
+        <v>2019</v>
+      </c>
+      <c r="H26">
+        <v>12</v>
+      </c>
+      <c r="I26">
+        <v>31</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+      <c r="K26">
+        <v>18</v>
+      </c>
+      <c r="L26" t="s">
+        <v>31</v>
+      </c>
+      <c r="M26" t="s">
+        <v>31</v>
+      </c>
+      <c r="N26" t="s">
+        <v>31</v>
+      </c>
+      <c r="O26" t="s">
+        <v>31</v>
+      </c>
+      <c r="P26" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>